<commit_message>
some bugfixes, and a third savegame
from supersandro2000
</commit_message>
<xml_diff>
--- a/Counter Calculations.xlsx
+++ b/Counter Calculations.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="77">
   <si>
     <t>Modules Installed</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t>Bird</t>
+  </si>
+  <si>
+    <t>SuperSandro2000</t>
+  </si>
+  <si>
+    <t>DyTech01</t>
   </si>
 </sst>
 </file>
@@ -973,17 +979,11 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1032,142 +1032,166 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="8" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="9" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="12" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="14" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="29" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="31" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="27" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="32" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="27" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="33" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="34" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="8" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="9" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="12" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="14" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="29" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="31" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="26" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="24" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="26" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="32" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="22" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="27" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="27" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="33" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="28" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="21" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="25" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="28" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="34" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="23" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1461,13 +1485,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="AT7" sqref="AT7"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AM5" sqref="AM5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -1518,1180 +1542,1291 @@
     <col min="49" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="35" customFormat="1" ht="37.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:48" s="30" customFormat="1" ht="37.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34" t="s">
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34" t="s">
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34" t="s">
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34" t="s">
+      <c r="AE1" s="50"/>
+      <c r="AF1" s="50"/>
+      <c r="AG1" s="50"/>
+      <c r="AH1" s="50"/>
+      <c r="AI1" s="50"/>
+      <c r="AJ1" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34" t="s">
+      <c r="AK1" s="50"/>
+      <c r="AL1" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
-      <c r="AO1" s="34"/>
-      <c r="AP1" s="34"/>
-      <c r="AQ1" s="34"/>
-      <c r="AR1" s="34"/>
-      <c r="AS1" s="34"/>
-      <c r="AT1" s="34"/>
-      <c r="AU1" s="34" t="s">
+      <c r="AM1" s="50"/>
+      <c r="AN1" s="50"/>
+      <c r="AO1" s="50"/>
+      <c r="AP1" s="50"/>
+      <c r="AQ1" s="50"/>
+      <c r="AR1" s="50"/>
+      <c r="AS1" s="50"/>
+      <c r="AT1" s="50"/>
+      <c r="AU1" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="AV1" s="34"/>
+      <c r="AV1" s="50"/>
     </row>
-    <row r="2" spans="1:48" s="36" customFormat="1" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:48" s="31" customFormat="1" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="36" t="s">
+      <c r="L2" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="M2" s="36" t="s">
+      <c r="M2" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="36" t="s">
+      <c r="N2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="O2" s="36" t="s">
+      <c r="O2" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="P2" s="36" t="s">
+      <c r="P2" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="Q2" s="36" t="s">
+      <c r="Q2" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="36" t="s">
+      <c r="R2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="36" t="s">
+      <c r="S2" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="T2" s="36" t="s">
+      <c r="T2" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="U2" s="36" t="s">
+      <c r="U2" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="V2" s="36" t="s">
+      <c r="V2" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="W2" s="36" t="s">
+      <c r="W2" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="X2" s="36" t="s">
+      <c r="X2" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="Y2" s="36" t="s">
+      <c r="Y2" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="Z2" s="36" t="s">
+      <c r="Z2" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="AA2" s="36" t="s">
+      <c r="AA2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="AB2" s="37" t="s">
+      <c r="AB2" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="36" t="s">
+      <c r="AC2" s="49"/>
+      <c r="AD2" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="AE2" s="36" t="s">
+      <c r="AE2" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="AF2" s="36" t="s">
+      <c r="AF2" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="AG2" s="36" t="s">
+      <c r="AG2" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="AH2" s="36" t="s">
+      <c r="AH2" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="AI2" s="36" t="s">
+      <c r="AI2" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="AJ2" s="37" t="s">
+      <c r="AJ2" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="AK2" s="37"/>
-      <c r="AL2" s="36" t="s">
+      <c r="AK2" s="49"/>
+      <c r="AL2" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="AM2" s="36" t="s">
+      <c r="AM2" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="AN2" s="36" t="s">
+      <c r="AN2" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="AO2" s="36" t="s">
+      <c r="AO2" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="AP2" s="36" t="s">
+      <c r="AP2" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="AQ2" s="36" t="s">
+      <c r="AQ2" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="AR2" s="36" t="s">
+      <c r="AR2" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="AS2" s="36" t="s">
+      <c r="AS2" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="AT2" s="36" t="s">
+      <c r="AT2" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="AU2" s="37" t="s">
+      <c r="AU2" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="AV2" s="37"/>
+      <c r="AV2" s="49"/>
     </row>
     <row r="3" spans="1:48" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="34">
         <v>23</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="14">
         <v>29</v>
       </c>
-      <c r="E3" s="43">
+      <c r="E3" s="36">
         <v>5</v>
       </c>
-      <c r="F3" s="63">
+      <c r="F3" s="45">
         <f>D3+(C3*60)+(E3/60)</f>
         <v>1409.0833333333333</v>
       </c>
-      <c r="G3" s="45">
+      <c r="G3" s="55">
         <v>4747</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="56">
         <v>5668</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="56">
         <v>245</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="56">
         <v>208</v>
       </c>
-      <c r="K3" s="16">
+      <c r="K3" s="56">
         <v>95</v>
       </c>
-      <c r="L3" s="16">
+      <c r="L3" s="56">
         <v>1</v>
       </c>
-      <c r="M3" s="16">
+      <c r="M3" s="56">
         <v>929</v>
       </c>
-      <c r="N3" s="16">
-        <v>0</v>
-      </c>
-      <c r="O3" s="16">
+      <c r="N3" s="56">
+        <v>0</v>
+      </c>
+      <c r="O3" s="56">
         <v>13343.5</v>
       </c>
-      <c r="P3" s="16">
+      <c r="P3" s="56">
         <v>44725.5</v>
       </c>
-      <c r="Q3" s="16">
+      <c r="Q3" s="56">
         <v>1257</v>
       </c>
-      <c r="R3" s="16">
+      <c r="R3" s="56">
         <v>1701</v>
       </c>
-      <c r="S3" s="16">
+      <c r="S3" s="56">
         <v>458</v>
       </c>
-      <c r="T3" s="16">
-        <v>0</v>
-      </c>
-      <c r="U3" s="16">
-        <v>0</v>
-      </c>
-      <c r="V3" s="16">
+      <c r="T3" s="56">
+        <v>0</v>
+      </c>
+      <c r="U3" s="56">
+        <v>0</v>
+      </c>
+      <c r="V3" s="56">
         <v>2127</v>
       </c>
-      <c r="W3" s="16">
-        <v>0</v>
-      </c>
-      <c r="X3" s="16">
+      <c r="W3" s="56">
+        <v>0</v>
+      </c>
+      <c r="X3" s="56">
         <v>300</v>
       </c>
-      <c r="Y3" s="16">
+      <c r="Y3" s="56">
         <v>601</v>
       </c>
-      <c r="Z3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="43">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="48">
+      <c r="Z3" s="56">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="57">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="58">
         <f>SUM(G3:AA3)</f>
         <v>76406</v>
       </c>
-      <c r="AC3" s="49"/>
-      <c r="AD3" s="41">
+      <c r="AC3" s="59"/>
+      <c r="AD3" s="60">
         <v>10230</v>
       </c>
-      <c r="AE3" s="16">
+      <c r="AE3" s="56">
         <v>4875</v>
       </c>
-      <c r="AF3" s="16">
+      <c r="AF3" s="56">
         <v>14106</v>
       </c>
-      <c r="AG3" s="16">
+      <c r="AG3" s="56">
         <v>4837</v>
       </c>
-      <c r="AH3" s="16">
+      <c r="AH3" s="56">
         <v>11595</v>
       </c>
-      <c r="AI3" s="43">
+      <c r="AI3" s="57">
         <v>3039</v>
       </c>
-      <c r="AJ3" s="48">
+      <c r="AJ3" s="58">
         <f>SUM(AD3:AI3)</f>
         <v>48682</v>
       </c>
-      <c r="AK3" s="49"/>
-      <c r="AL3" s="41">
+      <c r="AK3" s="59"/>
+      <c r="AL3" s="60">
         <v>2346</v>
       </c>
-      <c r="AM3" s="16">
+      <c r="AM3" s="56">
         <v>1192</v>
       </c>
-      <c r="AN3" s="16">
+      <c r="AN3" s="56">
         <v>654</v>
       </c>
-      <c r="AO3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="16">
+      <c r="AO3" s="56">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="56">
         <v>52</v>
       </c>
-      <c r="AQ3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="43">
-        <v>0</v>
-      </c>
-      <c r="AU3" s="48">
+      <c r="AQ3" s="56">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="56">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="56">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="57">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="58">
         <f>SUM(AL3:AT3)</f>
         <v>4244</v>
       </c>
-      <c r="AV3" s="49"/>
+      <c r="AV3" s="59"/>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="34">
         <v>33</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="14">
         <v>42</v>
       </c>
-      <c r="E4" s="43">
+      <c r="E4" s="36">
         <v>25</v>
       </c>
-      <c r="F4" s="64">
+      <c r="F4" s="46">
         <f t="shared" ref="F4:F12" si="0">D4+(C4*60)+(E4/60)</f>
         <v>2022.4166666666667</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="61">
         <v>10488</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="56">
         <v>38098</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="56">
         <v>1222</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="56">
         <v>953</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="56">
         <v>10</v>
       </c>
-      <c r="L4" s="16">
+      <c r="L4" s="56">
         <v>3</v>
       </c>
-      <c r="M4" s="16">
+      <c r="M4" s="56">
         <v>1469</v>
       </c>
-      <c r="N4" s="16">
-        <v>0</v>
-      </c>
-      <c r="O4" s="16">
+      <c r="N4" s="56">
+        <v>0</v>
+      </c>
+      <c r="O4" s="56">
         <v>44096.5</v>
       </c>
-      <c r="P4" s="16">
+      <c r="P4" s="56">
         <v>95559.5</v>
       </c>
-      <c r="Q4" s="16">
+      <c r="Q4" s="56">
         <v>814</v>
       </c>
-      <c r="R4" s="16">
+      <c r="R4" s="56">
         <v>1224</v>
       </c>
-      <c r="S4" s="16">
+      <c r="S4" s="56">
         <v>378</v>
       </c>
-      <c r="T4" s="16">
+      <c r="T4" s="56">
         <v>122</v>
       </c>
-      <c r="U4" s="16">
+      <c r="U4" s="56">
         <v>22</v>
       </c>
-      <c r="V4" s="16">
+      <c r="V4" s="56">
         <v>2795</v>
       </c>
-      <c r="W4" s="16">
+      <c r="W4" s="56">
         <v>981</v>
       </c>
-      <c r="X4" s="16">
+      <c r="X4" s="56">
         <v>1726</v>
       </c>
-      <c r="Y4" s="16">
+      <c r="Y4" s="56">
         <v>165</v>
       </c>
-      <c r="Z4" s="16">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="43">
+      <c r="Z4" s="56">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="57">
         <v>872</v>
       </c>
-      <c r="AB4" s="50">
+      <c r="AB4" s="62">
         <f>SUM(G4:AA4)</f>
         <v>200998</v>
       </c>
-      <c r="AC4" s="51"/>
-      <c r="AD4" s="41">
+      <c r="AC4" s="63"/>
+      <c r="AD4" s="60">
         <v>45467</v>
       </c>
-      <c r="AE4" s="16">
+      <c r="AE4" s="56">
         <v>115404</v>
       </c>
-      <c r="AF4" s="16">
+      <c r="AF4" s="56">
         <v>4490</v>
       </c>
-      <c r="AG4" s="16">
+      <c r="AG4" s="56">
         <v>61395</v>
       </c>
-      <c r="AH4" s="16">
+      <c r="AH4" s="56">
         <v>27289</v>
       </c>
-      <c r="AI4" s="43">
+      <c r="AI4" s="57">
         <v>4306</v>
       </c>
-      <c r="AJ4" s="50">
+      <c r="AJ4" s="62">
         <f>SUM(AD4:AI4)</f>
         <v>258351</v>
       </c>
-      <c r="AK4" s="51"/>
-      <c r="AL4" s="41">
+      <c r="AK4" s="63"/>
+      <c r="AL4" s="60">
         <v>19908</v>
       </c>
-      <c r="AM4" s="16">
+      <c r="AM4" s="56">
         <v>14511</v>
       </c>
-      <c r="AN4" s="16">
+      <c r="AN4" s="56">
         <v>10358</v>
       </c>
-      <c r="AO4" s="16">
-        <v>0</v>
-      </c>
-      <c r="AP4" s="16">
+      <c r="AO4" s="56">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="56">
         <v>4951</v>
       </c>
-      <c r="AQ4" s="16">
+      <c r="AQ4" s="56">
         <v>2094</v>
       </c>
-      <c r="AR4" s="16">
+      <c r="AR4" s="56">
         <v>426</v>
       </c>
-      <c r="AS4" s="16">
-        <v>0</v>
-      </c>
-      <c r="AT4" s="43">
-        <v>0</v>
-      </c>
-      <c r="AU4" s="50">
+      <c r="AS4" s="56">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="57">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="62">
         <f>SUM(AL4:AT4)</f>
         <v>52248</v>
       </c>
-      <c r="AV4" s="51"/>
+      <c r="AV4" s="63"/>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A5" s="58"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="64">
+      <c r="A5" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="34">
+        <v>8</v>
+      </c>
+      <c r="D5" s="14">
+        <v>30</v>
+      </c>
+      <c r="E5" s="36">
+        <v>24</v>
+      </c>
+      <c r="F5" s="46">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="46"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16"/>
-      <c r="W5" s="16"/>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="16"/>
-      <c r="AA5" s="43"/>
-      <c r="AB5" s="50">
+        <v>510.4</v>
+      </c>
+      <c r="G5" s="61">
+        <v>12266</v>
+      </c>
+      <c r="H5" s="56">
+        <v>9408.5</v>
+      </c>
+      <c r="I5" s="56">
+        <v>124</v>
+      </c>
+      <c r="J5" s="56">
+        <v>280</v>
+      </c>
+      <c r="K5" s="56">
+        <v>427</v>
+      </c>
+      <c r="L5" s="56">
+        <v>2</v>
+      </c>
+      <c r="M5" s="56">
+        <v>766</v>
+      </c>
+      <c r="N5" s="56">
+        <v>30</v>
+      </c>
+      <c r="O5" s="56">
+        <v>13089.5</v>
+      </c>
+      <c r="P5" s="56">
+        <v>53217.5</v>
+      </c>
+      <c r="Q5" s="56">
+        <v>1272</v>
+      </c>
+      <c r="R5" s="56">
+        <v>725</v>
+      </c>
+      <c r="S5" s="56">
+        <v>220</v>
+      </c>
+      <c r="T5" s="56">
+        <v>9</v>
+      </c>
+      <c r="U5" s="56">
+        <v>0</v>
+      </c>
+      <c r="V5" s="56">
+        <v>4613</v>
+      </c>
+      <c r="W5" s="56">
+        <v>153</v>
+      </c>
+      <c r="X5" s="56">
+        <v>900</v>
+      </c>
+      <c r="Y5" s="56">
+        <v>116</v>
+      </c>
+      <c r="Z5" s="56">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="57">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="62">
         <f t="shared" ref="AB5:AB11" si="1">SUM(G5:AA5)</f>
-        <v>0</v>
-      </c>
-      <c r="AC5" s="51"/>
-      <c r="AD5" s="41"/>
-      <c r="AE5" s="16"/>
-      <c r="AF5" s="16"/>
-      <c r="AG5" s="16"/>
-      <c r="AH5" s="16"/>
-      <c r="AI5" s="43"/>
-      <c r="AJ5" s="50">
+        <v>97618.5</v>
+      </c>
+      <c r="AC5" s="63"/>
+      <c r="AD5" s="60">
+        <v>11473</v>
+      </c>
+      <c r="AE5" s="56">
+        <v>7226</v>
+      </c>
+      <c r="AF5" s="56">
+        <v>758</v>
+      </c>
+      <c r="AG5" s="56">
+        <v>660</v>
+      </c>
+      <c r="AH5" s="56">
+        <v>5279</v>
+      </c>
+      <c r="AI5" s="57">
+        <v>3094</v>
+      </c>
+      <c r="AJ5" s="62">
         <f t="shared" ref="AJ5:AJ11" si="2">SUM(AD5:AI5)</f>
-        <v>0</v>
-      </c>
-      <c r="AK5" s="51"/>
-      <c r="AL5" s="41"/>
-      <c r="AM5" s="16"/>
-      <c r="AN5" s="16"/>
-      <c r="AO5" s="16"/>
-      <c r="AP5" s="16"/>
-      <c r="AQ5" s="16"/>
-      <c r="AR5" s="16"/>
-      <c r="AS5" s="16"/>
-      <c r="AT5" s="43"/>
-      <c r="AU5" s="50">
+        <v>28490</v>
+      </c>
+      <c r="AK5" s="63"/>
+      <c r="AL5" s="60">
+        <v>410</v>
+      </c>
+      <c r="AM5" s="56">
+        <v>188</v>
+      </c>
+      <c r="AN5" s="56">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="56">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="56">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="56">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="56">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="56">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="57">
+        <v>0</v>
+      </c>
+      <c r="AU5" s="62">
         <f t="shared" ref="AU5:AU11" si="3">SUM(AL5:AT5)</f>
-        <v>0</v>
-      </c>
-      <c r="AV5" s="51"/>
+        <v>598</v>
+      </c>
+      <c r="AV5" s="63"/>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A6" s="58"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="64">
+      <c r="A6" s="40"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6" s="46"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="16"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="16"/>
-      <c r="Z6" s="16"/>
-      <c r="AA6" s="43"/>
-      <c r="AB6" s="50">
+      <c r="G6" s="61"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="56"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="56"/>
+      <c r="Q6" s="56"/>
+      <c r="R6" s="56"/>
+      <c r="S6" s="56"/>
+      <c r="T6" s="56"/>
+      <c r="U6" s="56"/>
+      <c r="V6" s="56"/>
+      <c r="W6" s="56"/>
+      <c r="X6" s="56"/>
+      <c r="Y6" s="56"/>
+      <c r="Z6" s="56"/>
+      <c r="AA6" s="57"/>
+      <c r="AB6" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AC6" s="51"/>
-      <c r="AD6" s="41"/>
-      <c r="AE6" s="16"/>
-      <c r="AF6" s="16"/>
-      <c r="AG6" s="16"/>
-      <c r="AH6" s="16"/>
-      <c r="AI6" s="43"/>
-      <c r="AJ6" s="50">
+      <c r="AC6" s="63"/>
+      <c r="AD6" s="60"/>
+      <c r="AE6" s="56"/>
+      <c r="AF6" s="56"/>
+      <c r="AG6" s="56"/>
+      <c r="AH6" s="56"/>
+      <c r="AI6" s="57"/>
+      <c r="AJ6" s="62">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AK6" s="51"/>
-      <c r="AL6" s="41"/>
-      <c r="AM6" s="16"/>
-      <c r="AN6" s="16"/>
-      <c r="AO6" s="16"/>
-      <c r="AP6" s="16"/>
-      <c r="AQ6" s="16"/>
-      <c r="AR6" s="16"/>
-      <c r="AS6" s="16"/>
-      <c r="AT6" s="43"/>
-      <c r="AU6" s="50">
+      <c r="AK6" s="63"/>
+      <c r="AL6" s="60"/>
+      <c r="AM6" s="56"/>
+      <c r="AN6" s="56"/>
+      <c r="AO6" s="56"/>
+      <c r="AP6" s="56"/>
+      <c r="AQ6" s="56"/>
+      <c r="AR6" s="56"/>
+      <c r="AS6" s="56"/>
+      <c r="AT6" s="57"/>
+      <c r="AU6" s="62">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AV6" s="51"/>
+      <c r="AV6" s="63"/>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A7" s="58"/>
-      <c r="B7" s="59"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="64">
+      <c r="A7" s="40"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7" s="46"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="16"/>
-      <c r="Z7" s="16"/>
-      <c r="AA7" s="43"/>
-      <c r="AB7" s="50">
+      <c r="G7" s="61"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="56"/>
+      <c r="O7" s="56"/>
+      <c r="P7" s="56"/>
+      <c r="Q7" s="56"/>
+      <c r="R7" s="56"/>
+      <c r="S7" s="56"/>
+      <c r="T7" s="56"/>
+      <c r="U7" s="56"/>
+      <c r="V7" s="56"/>
+      <c r="W7" s="56"/>
+      <c r="X7" s="56"/>
+      <c r="Y7" s="56"/>
+      <c r="Z7" s="56"/>
+      <c r="AA7" s="57"/>
+      <c r="AB7" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AC7" s="51"/>
-      <c r="AD7" s="41"/>
-      <c r="AE7" s="16"/>
-      <c r="AF7" s="16"/>
-      <c r="AG7" s="16"/>
-      <c r="AH7" s="16"/>
-      <c r="AI7" s="43"/>
-      <c r="AJ7" s="50">
+      <c r="AC7" s="63"/>
+      <c r="AD7" s="60"/>
+      <c r="AE7" s="56"/>
+      <c r="AF7" s="56"/>
+      <c r="AG7" s="56"/>
+      <c r="AH7" s="56"/>
+      <c r="AI7" s="57"/>
+      <c r="AJ7" s="62">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AK7" s="51"/>
-      <c r="AL7" s="41"/>
-      <c r="AM7" s="16"/>
-      <c r="AN7" s="16"/>
-      <c r="AO7" s="16"/>
-      <c r="AP7" s="16"/>
-      <c r="AQ7" s="16"/>
-      <c r="AR7" s="16"/>
-      <c r="AS7" s="16"/>
-      <c r="AT7" s="43"/>
-      <c r="AU7" s="50">
+      <c r="AK7" s="63"/>
+      <c r="AL7" s="60"/>
+      <c r="AM7" s="56"/>
+      <c r="AN7" s="56"/>
+      <c r="AO7" s="56"/>
+      <c r="AP7" s="56"/>
+      <c r="AQ7" s="56"/>
+      <c r="AR7" s="56"/>
+      <c r="AS7" s="56"/>
+      <c r="AT7" s="57"/>
+      <c r="AU7" s="62">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AV7" s="51"/>
+      <c r="AV7" s="63"/>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A8" s="58"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="64">
+      <c r="A8" s="40"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="46"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
-      <c r="X8" s="16"/>
-      <c r="Y8" s="16"/>
-      <c r="Z8" s="16"/>
-      <c r="AA8" s="43"/>
-      <c r="AB8" s="50">
+      <c r="G8" s="61"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="56"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="56"/>
+      <c r="P8" s="56"/>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="56"/>
+      <c r="S8" s="56"/>
+      <c r="T8" s="56"/>
+      <c r="U8" s="56"/>
+      <c r="V8" s="56"/>
+      <c r="W8" s="56"/>
+      <c r="X8" s="56"/>
+      <c r="Y8" s="56"/>
+      <c r="Z8" s="56"/>
+      <c r="AA8" s="57"/>
+      <c r="AB8" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AC8" s="51"/>
-      <c r="AD8" s="41"/>
-      <c r="AE8" s="16"/>
-      <c r="AF8" s="16"/>
-      <c r="AG8" s="16"/>
-      <c r="AH8" s="16"/>
-      <c r="AI8" s="43"/>
-      <c r="AJ8" s="50">
+      <c r="AC8" s="63"/>
+      <c r="AD8" s="60"/>
+      <c r="AE8" s="56"/>
+      <c r="AF8" s="56"/>
+      <c r="AG8" s="56"/>
+      <c r="AH8" s="56"/>
+      <c r="AI8" s="57"/>
+      <c r="AJ8" s="62">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AK8" s="51"/>
-      <c r="AL8" s="41"/>
-      <c r="AM8" s="16"/>
-      <c r="AN8" s="16"/>
-      <c r="AO8" s="16"/>
-      <c r="AP8" s="16"/>
-      <c r="AQ8" s="16"/>
-      <c r="AR8" s="16"/>
-      <c r="AS8" s="16"/>
-      <c r="AT8" s="43"/>
-      <c r="AU8" s="50">
+      <c r="AK8" s="63"/>
+      <c r="AL8" s="60"/>
+      <c r="AM8" s="56"/>
+      <c r="AN8" s="56"/>
+      <c r="AO8" s="56"/>
+      <c r="AP8" s="56"/>
+      <c r="AQ8" s="56"/>
+      <c r="AR8" s="56"/>
+      <c r="AS8" s="56"/>
+      <c r="AT8" s="57"/>
+      <c r="AU8" s="62">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AV8" s="51"/>
+      <c r="AV8" s="63"/>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A9" s="58"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="64">
+      <c r="A9" s="40"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="46"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="16"/>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="16"/>
-      <c r="Z9" s="16"/>
-      <c r="AA9" s="43"/>
-      <c r="AB9" s="50">
+      <c r="G9" s="61"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="56"/>
+      <c r="S9" s="56"/>
+      <c r="T9" s="56"/>
+      <c r="U9" s="56"/>
+      <c r="V9" s="56"/>
+      <c r="W9" s="56"/>
+      <c r="X9" s="56"/>
+      <c r="Y9" s="56"/>
+      <c r="Z9" s="56"/>
+      <c r="AA9" s="57"/>
+      <c r="AB9" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AC9" s="51"/>
-      <c r="AD9" s="41"/>
-      <c r="AE9" s="16"/>
-      <c r="AF9" s="16"/>
-      <c r="AG9" s="16"/>
-      <c r="AH9" s="16"/>
-      <c r="AI9" s="43"/>
-      <c r="AJ9" s="50">
+      <c r="AC9" s="63"/>
+      <c r="AD9" s="60"/>
+      <c r="AE9" s="56"/>
+      <c r="AF9" s="56"/>
+      <c r="AG9" s="56"/>
+      <c r="AH9" s="56"/>
+      <c r="AI9" s="57"/>
+      <c r="AJ9" s="62">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AK9" s="51"/>
-      <c r="AL9" s="41"/>
-      <c r="AM9" s="16"/>
-      <c r="AN9" s="16"/>
-      <c r="AO9" s="16"/>
-      <c r="AP9" s="16"/>
-      <c r="AQ9" s="16"/>
-      <c r="AR9" s="16"/>
-      <c r="AS9" s="16"/>
-      <c r="AT9" s="43"/>
-      <c r="AU9" s="50">
+      <c r="AK9" s="63"/>
+      <c r="AL9" s="60"/>
+      <c r="AM9" s="56"/>
+      <c r="AN9" s="56"/>
+      <c r="AO9" s="56"/>
+      <c r="AP9" s="56"/>
+      <c r="AQ9" s="56"/>
+      <c r="AR9" s="56"/>
+      <c r="AS9" s="56"/>
+      <c r="AT9" s="57"/>
+      <c r="AU9" s="62">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AV9" s="51"/>
+      <c r="AV9" s="63"/>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A10" s="58"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="64">
+      <c r="A10" s="40"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="46"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="16"/>
-      <c r="T10" s="16"/>
-      <c r="U10" s="16"/>
-      <c r="V10" s="16"/>
-      <c r="W10" s="16"/>
-      <c r="X10" s="16"/>
-      <c r="Y10" s="16"/>
-      <c r="Z10" s="16"/>
-      <c r="AA10" s="43"/>
-      <c r="AB10" s="50">
+      <c r="G10" s="61"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="56"/>
+      <c r="P10" s="56"/>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="56"/>
+      <c r="S10" s="56"/>
+      <c r="T10" s="56"/>
+      <c r="U10" s="56"/>
+      <c r="V10" s="56"/>
+      <c r="W10" s="56"/>
+      <c r="X10" s="56"/>
+      <c r="Y10" s="56"/>
+      <c r="Z10" s="56"/>
+      <c r="AA10" s="57"/>
+      <c r="AB10" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AC10" s="51"/>
-      <c r="AD10" s="41"/>
-      <c r="AE10" s="16"/>
-      <c r="AF10" s="16"/>
-      <c r="AG10" s="16"/>
-      <c r="AH10" s="16"/>
-      <c r="AI10" s="43"/>
-      <c r="AJ10" s="50">
+      <c r="AC10" s="63"/>
+      <c r="AD10" s="60"/>
+      <c r="AE10" s="56"/>
+      <c r="AF10" s="56"/>
+      <c r="AG10" s="56"/>
+      <c r="AH10" s="56"/>
+      <c r="AI10" s="57"/>
+      <c r="AJ10" s="62">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AK10" s="51"/>
-      <c r="AL10" s="41"/>
-      <c r="AM10" s="16"/>
-      <c r="AN10" s="16"/>
-      <c r="AO10" s="16"/>
-      <c r="AP10" s="16"/>
-      <c r="AQ10" s="16"/>
-      <c r="AR10" s="16"/>
-      <c r="AS10" s="16"/>
-      <c r="AT10" s="43"/>
-      <c r="AU10" s="50">
+      <c r="AK10" s="63"/>
+      <c r="AL10" s="60"/>
+      <c r="AM10" s="56"/>
+      <c r="AN10" s="56"/>
+      <c r="AO10" s="56"/>
+      <c r="AP10" s="56"/>
+      <c r="AQ10" s="56"/>
+      <c r="AR10" s="56"/>
+      <c r="AS10" s="56"/>
+      <c r="AT10" s="57"/>
+      <c r="AU10" s="62">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AV10" s="51"/>
+      <c r="AV10" s="63"/>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A11" s="58"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="64">
+      <c r="A11" s="40"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" s="46"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="16"/>
-      <c r="V11" s="16"/>
-      <c r="W11" s="16"/>
-      <c r="X11" s="16"/>
-      <c r="Y11" s="16"/>
-      <c r="Z11" s="16"/>
-      <c r="AA11" s="43"/>
-      <c r="AB11" s="50">
+      <c r="G11" s="61"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="56"/>
+      <c r="P11" s="56"/>
+      <c r="Q11" s="56"/>
+      <c r="R11" s="56"/>
+      <c r="S11" s="56"/>
+      <c r="T11" s="56"/>
+      <c r="U11" s="56"/>
+      <c r="V11" s="56"/>
+      <c r="W11" s="56"/>
+      <c r="X11" s="56"/>
+      <c r="Y11" s="56"/>
+      <c r="Z11" s="56"/>
+      <c r="AA11" s="57"/>
+      <c r="AB11" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AC11" s="51"/>
-      <c r="AD11" s="41"/>
-      <c r="AE11" s="16"/>
-      <c r="AF11" s="16"/>
-      <c r="AG11" s="16"/>
-      <c r="AH11" s="16"/>
-      <c r="AI11" s="43"/>
-      <c r="AJ11" s="50">
+      <c r="AC11" s="63"/>
+      <c r="AD11" s="60"/>
+      <c r="AE11" s="56"/>
+      <c r="AF11" s="56"/>
+      <c r="AG11" s="56"/>
+      <c r="AH11" s="56"/>
+      <c r="AI11" s="57"/>
+      <c r="AJ11" s="62">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AK11" s="51"/>
-      <c r="AL11" s="41"/>
-      <c r="AM11" s="16"/>
-      <c r="AN11" s="16"/>
-      <c r="AO11" s="16"/>
-      <c r="AP11" s="16"/>
-      <c r="AQ11" s="16"/>
-      <c r="AR11" s="16"/>
-      <c r="AS11" s="16"/>
-      <c r="AT11" s="43"/>
-      <c r="AU11" s="50">
+      <c r="AK11" s="63"/>
+      <c r="AL11" s="60"/>
+      <c r="AM11" s="56"/>
+      <c r="AN11" s="56"/>
+      <c r="AO11" s="56"/>
+      <c r="AP11" s="56"/>
+      <c r="AQ11" s="56"/>
+      <c r="AR11" s="56"/>
+      <c r="AS11" s="56"/>
+      <c r="AT11" s="57"/>
+      <c r="AU11" s="62">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AV11" s="51"/>
+      <c r="AV11" s="63"/>
     </row>
     <row r="12" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="60"/>
-      <c r="B12" s="61"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="65">
+      <c r="A12" s="42"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G12" s="47"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="38"/>
-      <c r="S12" s="38"/>
-      <c r="T12" s="38"/>
-      <c r="U12" s="38"/>
-      <c r="V12" s="38"/>
-      <c r="W12" s="38"/>
-      <c r="X12" s="38"/>
-      <c r="Y12" s="38"/>
-      <c r="Z12" s="44"/>
-      <c r="AA12" s="44"/>
-      <c r="AB12" s="52">
+      <c r="G12" s="64"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="65"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="65"/>
+      <c r="N12" s="65"/>
+      <c r="O12" s="65"/>
+      <c r="P12" s="65"/>
+      <c r="Q12" s="65"/>
+      <c r="R12" s="65"/>
+      <c r="S12" s="65"/>
+      <c r="T12" s="65"/>
+      <c r="U12" s="65"/>
+      <c r="V12" s="65"/>
+      <c r="W12" s="65"/>
+      <c r="X12" s="65"/>
+      <c r="Y12" s="65"/>
+      <c r="Z12" s="66"/>
+      <c r="AA12" s="66"/>
+      <c r="AB12" s="67">
         <f>SUM(G12:AA12)</f>
         <v>0</v>
       </c>
-      <c r="AC12" s="53"/>
-      <c r="AD12" s="42"/>
-      <c r="AE12" s="38"/>
-      <c r="AF12" s="38"/>
-      <c r="AG12" s="38"/>
-      <c r="AH12" s="38"/>
-      <c r="AI12" s="44"/>
-      <c r="AJ12" s="52">
+      <c r="AC12" s="68"/>
+      <c r="AD12" s="69"/>
+      <c r="AE12" s="65"/>
+      <c r="AF12" s="65"/>
+      <c r="AG12" s="65"/>
+      <c r="AH12" s="65"/>
+      <c r="AI12" s="66"/>
+      <c r="AJ12" s="67">
         <f>SUM(AD12:AI12)</f>
         <v>0</v>
       </c>
-      <c r="AK12" s="53"/>
-      <c r="AL12" s="42"/>
-      <c r="AM12" s="38"/>
-      <c r="AN12" s="38"/>
-      <c r="AO12" s="38"/>
-      <c r="AP12" s="38"/>
-      <c r="AQ12" s="38"/>
-      <c r="AR12" s="38"/>
-      <c r="AS12" s="38"/>
-      <c r="AT12" s="44"/>
-      <c r="AU12" s="52">
+      <c r="AK12" s="68"/>
+      <c r="AL12" s="69"/>
+      <c r="AM12" s="65"/>
+      <c r="AN12" s="65"/>
+      <c r="AO12" s="65"/>
+      <c r="AP12" s="65"/>
+      <c r="AQ12" s="65"/>
+      <c r="AR12" s="65"/>
+      <c r="AS12" s="65"/>
+      <c r="AT12" s="66"/>
+      <c r="AU12" s="67">
         <f>SUM(AL12:AT12)</f>
         <v>0</v>
       </c>
-      <c r="AV12" s="53"/>
+      <c r="AV12" s="68"/>
     </row>
-    <row r="13" spans="1:48" s="40" customFormat="1" ht="48" thickTop="1" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A13" s="39" t="s">
+    <row r="13" spans="1:48" s="33" customFormat="1" ht="48" thickTop="1" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A13" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="40">
+      <c r="B13" s="48"/>
+      <c r="C13" s="44">
         <f>AVERAGE(C3:C12)</f>
-        <v>28</v>
-      </c>
-      <c r="D13" s="40">
+        <v>21.333333333333332</v>
+      </c>
+      <c r="D13" s="44">
         <f t="shared" ref="D13:AA13" si="4">AVERAGE(D3:D12)</f>
-        <v>35.5</v>
-      </c>
-      <c r="E13" s="40">
+        <v>33.666666666666664</v>
+      </c>
+      <c r="E13" s="44">
         <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="F13" s="62">
+        <v>18</v>
+      </c>
+      <c r="F13" s="44">
         <f>AVERAGE(F3:F4)</f>
         <v>1715.75</v>
       </c>
-      <c r="G13" s="40">
+      <c r="G13" s="44">
         <f t="shared" si="4"/>
-        <v>7617.5</v>
-      </c>
-      <c r="H13" s="40">
+        <v>9167</v>
+      </c>
+      <c r="H13" s="44">
         <f t="shared" si="4"/>
-        <v>21883</v>
-      </c>
-      <c r="I13" s="40">
+        <v>17724.833333333332</v>
+      </c>
+      <c r="I13" s="44">
         <f t="shared" si="4"/>
-        <v>733.5</v>
-      </c>
-      <c r="J13" s="40">
+        <v>530.33333333333337</v>
+      </c>
+      <c r="J13" s="44">
         <f t="shared" si="4"/>
-        <v>580.5</v>
-      </c>
-      <c r="K13" s="40">
+        <v>480.33333333333331</v>
+      </c>
+      <c r="K13" s="44">
         <f t="shared" si="4"/>
-        <v>52.5</v>
-      </c>
-      <c r="L13" s="40">
+        <v>177.33333333333334</v>
+      </c>
+      <c r="L13" s="44">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="M13" s="40">
+      <c r="M13" s="44">
         <f t="shared" si="4"/>
-        <v>1199</v>
-      </c>
-      <c r="N13" s="40">
+        <v>1054.6666666666667</v>
+      </c>
+      <c r="N13" s="44">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="40">
+        <v>10</v>
+      </c>
+      <c r="O13" s="44">
         <f t="shared" si="4"/>
-        <v>28720</v>
-      </c>
-      <c r="P13" s="40">
+        <v>23509.833333333332</v>
+      </c>
+      <c r="P13" s="44">
         <f t="shared" si="4"/>
-        <v>70142.5</v>
-      </c>
-      <c r="Q13" s="40">
+        <v>64500.833333333336</v>
+      </c>
+      <c r="Q13" s="44">
         <f t="shared" si="4"/>
-        <v>1035.5</v>
-      </c>
-      <c r="R13" s="40">
+        <v>1114.3333333333333</v>
+      </c>
+      <c r="R13" s="44">
         <f t="shared" si="4"/>
-        <v>1462.5</v>
-      </c>
-      <c r="S13" s="40">
+        <v>1216.6666666666667</v>
+      </c>
+      <c r="S13" s="44">
         <f t="shared" si="4"/>
-        <v>418</v>
-      </c>
-      <c r="T13" s="40">
+        <v>352</v>
+      </c>
+      <c r="T13" s="44">
         <f t="shared" si="4"/>
-        <v>61</v>
-      </c>
-      <c r="U13" s="40">
+        <v>43.666666666666664</v>
+      </c>
+      <c r="U13" s="44">
         <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="V13" s="40">
+        <v>7.333333333333333</v>
+      </c>
+      <c r="V13" s="44">
         <f t="shared" si="4"/>
-        <v>2461</v>
-      </c>
-      <c r="W13" s="40">
+        <v>3178.3333333333335</v>
+      </c>
+      <c r="W13" s="44">
         <f t="shared" si="4"/>
-        <v>490.5</v>
-      </c>
-      <c r="X13" s="40">
+        <v>378</v>
+      </c>
+      <c r="X13" s="44">
         <f t="shared" si="4"/>
-        <v>1013</v>
-      </c>
-      <c r="Y13" s="40">
+        <v>975.33333333333337</v>
+      </c>
+      <c r="Y13" s="44">
         <f t="shared" si="4"/>
-        <v>383</v>
-      </c>
-      <c r="Z13" s="40">
+        <v>294</v>
+      </c>
+      <c r="Z13" s="44">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AA13" s="40">
+      <c r="AA13" s="44">
         <f t="shared" si="4"/>
-        <v>436</v>
-      </c>
-      <c r="AB13" s="54">
+        <v>290.66666666666669</v>
+      </c>
+      <c r="AB13" s="70">
         <f>AVERAGE(AB3:AC4)</f>
         <v>138702</v>
       </c>
-      <c r="AC13" s="55"/>
-      <c r="AD13" s="40">
+      <c r="AC13" s="71"/>
+      <c r="AD13" s="44">
         <f>AVERAGE(AD3:AD12)</f>
-        <v>27848.5</v>
-      </c>
-      <c r="AE13" s="40">
+        <v>22390</v>
+      </c>
+      <c r="AE13" s="44">
         <f t="shared" ref="AE13:AI13" si="5">AVERAGE(AE3:AE12)</f>
-        <v>60139.5</v>
-      </c>
-      <c r="AF13" s="40">
+        <v>42501.666666666664</v>
+      </c>
+      <c r="AF13" s="44">
         <f t="shared" si="5"/>
-        <v>9298</v>
-      </c>
-      <c r="AG13" s="40">
+        <v>6451.333333333333</v>
+      </c>
+      <c r="AG13" s="44">
         <f t="shared" si="5"/>
-        <v>33116</v>
-      </c>
-      <c r="AH13" s="40">
+        <v>22297.333333333332</v>
+      </c>
+      <c r="AH13" s="44">
         <f t="shared" si="5"/>
-        <v>19442</v>
-      </c>
-      <c r="AI13" s="40">
+        <v>14721</v>
+      </c>
+      <c r="AI13" s="44">
         <f t="shared" si="5"/>
-        <v>3672.5</v>
-      </c>
-      <c r="AJ13" s="54">
+        <v>3479.6666666666665</v>
+      </c>
+      <c r="AJ13" s="70">
         <f>AVERAGE(AJ3:AK4)</f>
         <v>153516.5</v>
       </c>
-      <c r="AK13" s="55"/>
-      <c r="AL13" s="40">
+      <c r="AK13" s="71"/>
+      <c r="AL13" s="44">
         <f>AVERAGE(AL3:AL12)</f>
-        <v>11127</v>
-      </c>
-      <c r="AM13" s="40">
+        <v>7554.666666666667</v>
+      </c>
+      <c r="AM13" s="44">
         <f t="shared" ref="AM13:AT13" si="6">AVERAGE(AM3:AM12)</f>
-        <v>7851.5</v>
-      </c>
-      <c r="AN13" s="40">
+        <v>5297</v>
+      </c>
+      <c r="AN13" s="44">
         <f t="shared" si="6"/>
-        <v>5506</v>
-      </c>
-      <c r="AO13" s="40">
+        <v>3670.6666666666665</v>
+      </c>
+      <c r="AO13" s="44">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AP13" s="40">
+      <c r="AP13" s="44">
         <f t="shared" si="6"/>
-        <v>2501.5</v>
-      </c>
-      <c r="AQ13" s="40">
+        <v>1667.6666666666667</v>
+      </c>
+      <c r="AQ13" s="44">
         <f t="shared" si="6"/>
-        <v>1047</v>
-      </c>
-      <c r="AR13" s="40">
+        <v>698</v>
+      </c>
+      <c r="AR13" s="44">
         <f t="shared" si="6"/>
-        <v>213</v>
-      </c>
-      <c r="AS13" s="40">
+        <v>142</v>
+      </c>
+      <c r="AS13" s="44">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AT13" s="40">
+      <c r="AT13" s="44">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AU13" s="54">
+      <c r="AU13" s="70">
         <f>AVERAGE(AU3:AV4)</f>
         <v>28246</v>
       </c>
-      <c r="AV13" s="55"/>
+      <c r="AV13" s="71"/>
     </row>
     <row r="14" spans="1:48" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AI1"/>
+    <mergeCell ref="AJ9:AK9"/>
+    <mergeCell ref="AJ10:AK10"/>
+    <mergeCell ref="AJ11:AK11"/>
+    <mergeCell ref="AL1:AT1"/>
+    <mergeCell ref="AU1:AV1"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="AJ4:AK4"/>
+    <mergeCell ref="AJ5:AK5"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AU7:AV7"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="AJ6:AK6"/>
+    <mergeCell ref="AJ7:AK7"/>
+    <mergeCell ref="AU2:AV2"/>
+    <mergeCell ref="AU3:AV3"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AU6:AV6"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="AB13:AC13"/>
     <mergeCell ref="AJ13:AK13"/>
@@ -2707,38 +2842,10 @@
     <mergeCell ref="AB9:AC9"/>
     <mergeCell ref="AB10:AC10"/>
     <mergeCell ref="AB11:AC11"/>
-    <mergeCell ref="AU2:AV2"/>
-    <mergeCell ref="AU3:AV3"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="AU6:AV6"/>
-    <mergeCell ref="AU7:AV7"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="AJ6:AK6"/>
-    <mergeCell ref="AJ7:AK7"/>
     <mergeCell ref="AJ8:AK8"/>
-    <mergeCell ref="AJ9:AK9"/>
-    <mergeCell ref="AJ10:AK10"/>
-    <mergeCell ref="AJ11:AK11"/>
-    <mergeCell ref="AL1:AT1"/>
-    <mergeCell ref="AU1:AV1"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="AJ4:AK4"/>
-    <mergeCell ref="AJ5:AK5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AD1:AI1"/>
-    <mergeCell ref="AJ1:AK1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2809,379 +2916,379 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="A1" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
     </row>
     <row r="2" spans="1:18" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
     </row>
     <row r="3" spans="1:18" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="26">
         <v>1</v>
       </c>
-      <c r="C4" s="26">
-        <v>0</v>
-      </c>
-      <c r="D4" s="26">
-        <v>0</v>
-      </c>
-      <c r="E4" s="31">
+      <c r="C4" s="22">
+        <v>0</v>
+      </c>
+      <c r="D4" s="22">
+        <v>0</v>
+      </c>
+      <c r="E4" s="27">
         <v>1</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="27">
         <v>1</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="27">
         <v>1</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="27">
         <v>1</v>
       </c>
-      <c r="I4" s="26">
-        <v>0</v>
-      </c>
-      <c r="J4" s="31">
+      <c r="I4" s="22">
+        <v>0</v>
+      </c>
+      <c r="J4" s="27">
         <v>1</v>
       </c>
-      <c r="K4" s="31">
+      <c r="K4" s="27">
         <v>1</v>
       </c>
-      <c r="L4" s="31">
+      <c r="L4" s="27">
         <v>1</v>
       </c>
-      <c r="M4" s="31">
+      <c r="M4" s="27">
         <v>1</v>
       </c>
-      <c r="N4" s="31">
+      <c r="N4" s="27">
         <v>1</v>
       </c>
-      <c r="O4" s="32">
+      <c r="O4" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="25">
         <v>1</v>
       </c>
-      <c r="C5" s="27">
-        <v>0</v>
-      </c>
-      <c r="D5" s="27">
-        <v>0</v>
-      </c>
-      <c r="E5" s="28">
+      <c r="C5" s="23">
+        <v>0</v>
+      </c>
+      <c r="D5" s="23">
+        <v>0</v>
+      </c>
+      <c r="E5" s="24">
         <v>1</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="24">
         <v>1</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="24">
         <v>1</v>
       </c>
-      <c r="H5" s="27">
-        <v>0</v>
-      </c>
-      <c r="I5" s="27">
-        <v>0</v>
-      </c>
-      <c r="J5" s="28">
+      <c r="H5" s="23">
+        <v>0</v>
+      </c>
+      <c r="I5" s="23">
+        <v>0</v>
+      </c>
+      <c r="J5" s="24">
         <v>1</v>
       </c>
-      <c r="K5" s="28">
+      <c r="K5" s="24">
         <v>1</v>
       </c>
-      <c r="L5" s="28">
+      <c r="L5" s="24">
         <v>1</v>
       </c>
-      <c r="M5" s="28">
+      <c r="M5" s="24">
         <v>1</v>
       </c>
-      <c r="N5" s="28">
+      <c r="N5" s="24">
         <v>1</v>
       </c>
-      <c r="O5" s="33">
+      <c r="O5" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="11"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="9"/>
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="11"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="9"/>
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="11"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="9"/>
     </row>
     <row r="9" spans="1:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="11"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="9"/>
     </row>
     <row r="10" spans="1:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="11"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="9"/>
     </row>
     <row r="11" spans="1:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="11"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="9"/>
     </row>
     <row r="12" spans="1:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="11"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="9"/>
     </row>
     <row r="13" spans="1:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="8"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="14"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="12"/>
     </row>
     <row r="14" spans="1:18" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="15">
         <f>SUM(B4:B13)</f>
         <v>2</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="16">
         <f t="shared" ref="C14:O14" si="0">SUM(C4:C13)</f>
         <v>0</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="16">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="16">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="16">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="16">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I14" s="18">
+      <c r="I14" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="16">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="K14" s="18">
+      <c r="K14" s="16">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="L14" s="18">
+      <c r="L14" s="16">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="M14" s="18">
+      <c r="M14" s="16">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="N14" s="18">
+      <c r="N14" s="16">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="O14" s="19">
+      <c r="O14" s="17">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -3256,10 +3363,10 @@
     </row>
     <row r="19" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="21"/>
+      <c r="C19" s="54"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -3273,13 +3380,13 @@
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E20" s="1"/>
@@ -3295,13 +3402,13 @@
       <c r="O20" s="1"/>
     </row>
     <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="24">
+      <c r="B21" s="20">
         <v>1</v>
       </c>
-      <c r="C21" s="25">
-        <v>0</v>
-      </c>
-      <c r="D21" s="15" t="s">
+      <c r="C21" s="21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="13" t="s">
         <v>22</v>
       </c>
       <c r="E21" s="1"/>

</xml_diff>